<commit_message>
Optimized for NAND implementation
</commit_message>
<xml_diff>
--- a/Documentation/Monty08.xlsx
+++ b/Documentation/Monty08.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\CPU_8Bit\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE89ABB3-40FB-4F42-8BAE-BAE94EB4264D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D57FE8-E9B1-497C-BBA2-D56538434990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{5BA4E079-EFAB-4B55-B322-C6522B3056FF}"/>
+    <workbookView xWindow="38280" yWindow="3585" windowWidth="29040" windowHeight="16440" xr2:uid="{5BA4E079-EFAB-4B55-B322-C6522B3056FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Control-Unit" sheetId="1" r:id="rId1"/>
@@ -2902,6 +2902,12 @@
     <xf numFmtId="0" fontId="0" fillId="26" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3063,12 +3069,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3441,8 +3441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0373F33-972A-4E8D-B1CE-9C5EF0708B27}">
   <dimension ref="A2:AI157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA51" sqref="AA51"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3470,50 +3470,50 @@
     </row>
     <row r="4" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="247" t="s">
+      <c r="C5" s="249" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="248"/>
-      <c r="E5" s="248"/>
-      <c r="F5" s="248"/>
-      <c r="G5" s="248"/>
-      <c r="H5" s="248"/>
-      <c r="I5" s="248"/>
-      <c r="J5" s="248"/>
-      <c r="K5" s="248"/>
-      <c r="L5" s="249"/>
+      <c r="D5" s="250"/>
+      <c r="E5" s="250"/>
+      <c r="F5" s="250"/>
+      <c r="G5" s="250"/>
+      <c r="H5" s="250"/>
+      <c r="I5" s="250"/>
+      <c r="J5" s="250"/>
+      <c r="K5" s="250"/>
+      <c r="L5" s="251"/>
       <c r="M5" s="123"/>
-      <c r="N5" s="261" t="s">
+      <c r="N5" s="263" t="s">
         <v>85</v>
       </c>
-      <c r="O5" s="261"/>
-      <c r="P5" s="261"/>
-      <c r="Q5" s="261"/>
-      <c r="R5" s="261"/>
-      <c r="S5" s="261"/>
-      <c r="T5" s="261"/>
-      <c r="U5" s="261"/>
-      <c r="V5" s="261"/>
-      <c r="W5" s="261"/>
-      <c r="X5" s="261"/>
-      <c r="Y5" s="261"/>
-      <c r="Z5" s="261"/>
-      <c r="AA5" s="261"/>
-      <c r="AB5" s="261"/>
-      <c r="AC5" s="262"/>
-      <c r="AD5" s="245"/>
+      <c r="O5" s="263"/>
+      <c r="P5" s="263"/>
+      <c r="Q5" s="263"/>
+      <c r="R5" s="263"/>
+      <c r="S5" s="263"/>
+      <c r="T5" s="263"/>
+      <c r="U5" s="263"/>
+      <c r="V5" s="263"/>
+      <c r="W5" s="263"/>
+      <c r="X5" s="263"/>
+      <c r="Y5" s="263"/>
+      <c r="Z5" s="263"/>
+      <c r="AA5" s="263"/>
+      <c r="AB5" s="263"/>
+      <c r="AC5" s="264"/>
+      <c r="AD5" s="247"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="C6" s="250"/>
-      <c r="D6" s="251"/>
-      <c r="E6" s="251"/>
-      <c r="F6" s="251"/>
-      <c r="G6" s="251"/>
-      <c r="H6" s="251"/>
-      <c r="I6" s="251"/>
-      <c r="J6" s="251"/>
-      <c r="K6" s="251"/>
-      <c r="L6" s="252"/>
+      <c r="C6" s="252"/>
+      <c r="D6" s="253"/>
+      <c r="E6" s="253"/>
+      <c r="F6" s="253"/>
+      <c r="G6" s="253"/>
+      <c r="H6" s="253"/>
+      <c r="I6" s="253"/>
+      <c r="J6" s="253"/>
+      <c r="K6" s="253"/>
+      <c r="L6" s="254"/>
       <c r="M6" s="13"/>
       <c r="N6" s="4">
         <v>0</v>
@@ -3563,7 +3563,7 @@
       <c r="AC6" s="124">
         <v>15</v>
       </c>
-      <c r="AD6" s="246"/>
+      <c r="AD6" s="248"/>
       <c r="AE6" s="4"/>
       <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
@@ -3571,11 +3571,11 @@
       <c r="AI6" s="2"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="C7" s="253"/>
-      <c r="D7" s="254"/>
-      <c r="E7" s="254"/>
-      <c r="F7" s="254"/>
-      <c r="G7" s="254"/>
+      <c r="C7" s="255"/>
+      <c r="D7" s="256"/>
+      <c r="E7" s="256"/>
+      <c r="F7" s="256"/>
+      <c r="G7" s="256"/>
       <c r="H7" s="240"/>
       <c r="I7" s="24" t="s">
         <v>70</v>
@@ -3586,12 +3586,12 @@
       <c r="K7" s="18"/>
       <c r="L7" s="25"/>
       <c r="M7" s="121"/>
-      <c r="N7" s="263"/>
-      <c r="O7" s="263"/>
-      <c r="P7" s="263"/>
-      <c r="Q7" s="263"/>
-      <c r="R7" s="263"/>
-      <c r="S7" s="263"/>
+      <c r="N7" s="265"/>
+      <c r="O7" s="265"/>
+      <c r="P7" s="265"/>
+      <c r="Q7" s="265"/>
+      <c r="R7" s="265"/>
+      <c r="S7" s="265"/>
       <c r="T7" s="5" t="s">
         <v>113</v>
       </c>
@@ -3614,61 +3614,61 @@
       <c r="AA7" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="AB7" s="264" t="s">
+      <c r="AB7" s="266" t="s">
         <v>119</v>
       </c>
-      <c r="AC7" s="265"/>
-      <c r="AD7" s="246"/>
+      <c r="AC7" s="267"/>
+      <c r="AD7" s="248"/>
       <c r="AE7" s="2"/>
       <c r="AF7" s="3"/>
       <c r="AG7" s="3"/>
       <c r="AH7" s="2"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="C8" s="255" t="s">
+      <c r="C8" s="257" t="s">
         <v>329</v>
       </c>
-      <c r="D8" s="256"/>
-      <c r="E8" s="256"/>
-      <c r="F8" s="256"/>
-      <c r="G8" s="256"/>
+      <c r="D8" s="258"/>
+      <c r="E8" s="258"/>
+      <c r="F8" s="258"/>
+      <c r="G8" s="258"/>
       <c r="H8" s="40" t="s">
         <v>348</v>
       </c>
-      <c r="I8" s="257" t="s">
+      <c r="I8" s="259" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="258"/>
-      <c r="K8" s="258"/>
-      <c r="L8" s="259"/>
-      <c r="M8" s="260" t="s">
-        <v>1</v>
-      </c>
-      <c r="N8" s="260"/>
-      <c r="O8" s="260"/>
-      <c r="P8" s="260"/>
-      <c r="Q8" s="260"/>
-      <c r="R8" s="260"/>
-      <c r="S8" s="260"/>
-      <c r="T8" s="269" t="s">
+      <c r="J8" s="260"/>
+      <c r="K8" s="260"/>
+      <c r="L8" s="261"/>
+      <c r="M8" s="262" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="262"/>
+      <c r="O8" s="262"/>
+      <c r="P8" s="262"/>
+      <c r="Q8" s="262"/>
+      <c r="R8" s="262"/>
+      <c r="S8" s="262"/>
+      <c r="T8" s="271" t="s">
         <v>122</v>
       </c>
-      <c r="U8" s="269"/>
-      <c r="V8" s="270" t="s">
+      <c r="U8" s="271"/>
+      <c r="V8" s="272" t="s">
         <v>123</v>
       </c>
-      <c r="W8" s="270"/>
-      <c r="X8" s="270"/>
-      <c r="Y8" s="270"/>
-      <c r="Z8" s="268" t="s">
+      <c r="W8" s="272"/>
+      <c r="X8" s="272"/>
+      <c r="Y8" s="272"/>
+      <c r="Z8" s="270" t="s">
         <v>120</v>
       </c>
-      <c r="AA8" s="268"/>
-      <c r="AB8" s="266" t="s">
+      <c r="AA8" s="270"/>
+      <c r="AB8" s="268" t="s">
         <v>121</v>
       </c>
-      <c r="AC8" s="267"/>
-      <c r="AD8" s="246"/>
+      <c r="AC8" s="269"/>
+      <c r="AD8" s="248"/>
       <c r="AE8" s="118"/>
       <c r="AF8" s="118"/>
       <c r="AG8" s="118"/>
@@ -8183,52 +8183,52 @@
       <c r="M54" s="13">
         <v>1</v>
       </c>
-      <c r="N54" s="300">
-        <v>0</v>
-      </c>
-      <c r="O54" s="300">
-        <v>0</v>
-      </c>
-      <c r="P54" s="300">
-        <v>0</v>
-      </c>
-      <c r="Q54" s="300">
-        <v>0</v>
-      </c>
-      <c r="R54" s="300">
+      <c r="N54" s="245">
+        <v>0</v>
+      </c>
+      <c r="O54" s="245">
+        <v>0</v>
+      </c>
+      <c r="P54" s="245">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="245">
+        <v>0</v>
+      </c>
+      <c r="R54" s="245">
         <v>0</v>
       </c>
       <c r="S54" s="244">
         <v>0</v>
       </c>
-      <c r="T54" s="300">
+      <c r="T54" s="245">
         <v>1</v>
       </c>
       <c r="U54" s="244">
         <v>0</v>
       </c>
-      <c r="V54" s="300">
-        <v>1</v>
-      </c>
-      <c r="W54" s="300">
-        <v>1</v>
-      </c>
-      <c r="X54" s="300">
+      <c r="V54" s="245">
+        <v>1</v>
+      </c>
+      <c r="W54" s="245">
+        <v>1</v>
+      </c>
+      <c r="X54" s="245">
         <v>0</v>
       </c>
       <c r="Y54" s="244">
         <v>1</v>
       </c>
-      <c r="Z54" s="300">
+      <c r="Z54" s="245">
         <v>0</v>
       </c>
       <c r="AA54" s="244">
         <v>0</v>
       </c>
-      <c r="AB54" s="300">
-        <v>1</v>
-      </c>
-      <c r="AC54" s="301">
+      <c r="AB54" s="245">
+        <v>1</v>
+      </c>
+      <c r="AC54" s="246">
         <v>1</v>
       </c>
       <c r="AD54" s="173" t="str">
@@ -8281,52 +8281,52 @@
       <c r="M55" s="13">
         <v>1</v>
       </c>
-      <c r="N55" s="300">
-        <v>0</v>
-      </c>
-      <c r="O55" s="300">
-        <v>0</v>
-      </c>
-      <c r="P55" s="300">
-        <v>0</v>
-      </c>
-      <c r="Q55" s="300">
-        <v>0</v>
-      </c>
-      <c r="R55" s="300">
+      <c r="N55" s="245">
+        <v>0</v>
+      </c>
+      <c r="O55" s="245">
+        <v>0</v>
+      </c>
+      <c r="P55" s="245">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="245">
+        <v>0</v>
+      </c>
+      <c r="R55" s="245">
         <v>0</v>
       </c>
       <c r="S55" s="244">
         <v>0</v>
       </c>
-      <c r="T55" s="300">
+      <c r="T55" s="245">
         <v>1</v>
       </c>
       <c r="U55" s="244">
         <v>1</v>
       </c>
-      <c r="V55" s="300">
-        <v>1</v>
-      </c>
-      <c r="W55" s="300">
-        <v>0</v>
-      </c>
-      <c r="X55" s="300">
+      <c r="V55" s="245">
+        <v>1</v>
+      </c>
+      <c r="W55" s="245">
+        <v>0</v>
+      </c>
+      <c r="X55" s="245">
         <v>0</v>
       </c>
       <c r="Y55" s="244">
         <v>1</v>
       </c>
-      <c r="Z55" s="300">
+      <c r="Z55" s="245">
         <v>0</v>
       </c>
       <c r="AA55" s="244">
         <v>0</v>
       </c>
-      <c r="AB55" s="300">
-        <v>1</v>
-      </c>
-      <c r="AC55" s="301">
+      <c r="AB55" s="245">
+        <v>1</v>
+      </c>
+      <c r="AC55" s="246">
         <v>1</v>
       </c>
       <c r="AD55" s="173" t="str">
@@ -15122,61 +15122,61 @@
       <c r="F5" s="163" t="s">
         <v>209</v>
       </c>
-      <c r="G5" s="271" t="s">
+      <c r="G5" s="273" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="6" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F6" s="162"/>
-      <c r="G6" s="272"/>
+      <c r="G6" s="274"/>
     </row>
     <row r="7" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F7" s="162"/>
-      <c r="G7" s="272"/>
+      <c r="G7" s="274"/>
     </row>
     <row r="8" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F8" s="162"/>
-      <c r="G8" s="272"/>
+      <c r="G8" s="274"/>
     </row>
     <row r="9" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F9" s="162"/>
-      <c r="G9" s="272"/>
+      <c r="G9" s="274"/>
     </row>
     <row r="10" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F10" s="162"/>
-      <c r="G10" s="272"/>
+      <c r="G10" s="274"/>
     </row>
     <row r="11" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F11" s="162"/>
-      <c r="G11" s="272"/>
+      <c r="G11" s="274"/>
     </row>
     <row r="12" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F12" s="162"/>
-      <c r="G12" s="272"/>
+      <c r="G12" s="274"/>
     </row>
     <row r="13" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F13" s="162"/>
-      <c r="G13" s="272"/>
+      <c r="G13" s="274"/>
     </row>
     <row r="14" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F14" s="162"/>
-      <c r="G14" s="272"/>
+      <c r="G14" s="274"/>
     </row>
     <row r="15" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F15" s="162"/>
-      <c r="G15" s="272"/>
+      <c r="G15" s="274"/>
     </row>
     <row r="16" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F16" s="164" t="s">
         <v>213</v>
       </c>
-      <c r="G16" s="273"/>
+      <c r="G16" s="275"/>
     </row>
     <row r="17" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F17" s="162" t="s">
         <v>210</v>
       </c>
-      <c r="G17" s="274" t="s">
+      <c r="G17" s="276" t="s">
         <v>212</v>
       </c>
     </row>
@@ -15184,83 +15184,83 @@
       <c r="F18" s="164" t="s">
         <v>214</v>
       </c>
-      <c r="G18" s="275"/>
+      <c r="G18" s="277"/>
     </row>
     <row r="19" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F19" s="162" t="s">
         <v>215</v>
       </c>
-      <c r="G19" s="276" t="s">
+      <c r="G19" s="278" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="20" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F20" s="162"/>
-      <c r="G20" s="277"/>
+      <c r="G20" s="279"/>
     </row>
     <row r="21" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F21" s="162"/>
-      <c r="G21" s="277"/>
+      <c r="G21" s="279"/>
     </row>
     <row r="22" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F22" s="164" t="s">
         <v>216</v>
       </c>
-      <c r="G22" s="278"/>
+      <c r="G22" s="280"/>
     </row>
     <row r="23" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F23" s="162" t="s">
         <v>218</v>
       </c>
-      <c r="G23" s="279" t="s">
+      <c r="G23" s="281" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="24" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F24" s="162"/>
-      <c r="G24" s="280"/>
+      <c r="G24" s="282"/>
     </row>
     <row r="25" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F25" s="162"/>
-      <c r="G25" s="280"/>
+      <c r="G25" s="282"/>
     </row>
     <row r="26" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F26" s="162"/>
-      <c r="G26" s="280"/>
+      <c r="G26" s="282"/>
     </row>
     <row r="27" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F27" s="162"/>
-      <c r="G27" s="280"/>
+      <c r="G27" s="282"/>
     </row>
     <row r="28" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F28" s="162"/>
-      <c r="G28" s="280"/>
+      <c r="G28" s="282"/>
     </row>
     <row r="29" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F29" s="162"/>
-      <c r="G29" s="280"/>
+      <c r="G29" s="282"/>
     </row>
     <row r="30" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F30" s="162"/>
-      <c r="G30" s="280"/>
+      <c r="G30" s="282"/>
     </row>
     <row r="31" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F31" s="162"/>
-      <c r="G31" s="280"/>
+      <c r="G31" s="282"/>
     </row>
     <row r="32" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F32" s="162"/>
-      <c r="G32" s="280"/>
+      <c r="G32" s="282"/>
     </row>
     <row r="33" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F33" s="162"/>
-      <c r="G33" s="280"/>
+      <c r="G33" s="282"/>
     </row>
     <row r="34" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F34" s="164" t="s">
         <v>219</v>
       </c>
-      <c r="G34" s="281"/>
+      <c r="G34" s="283"/>
     </row>
     <row r="35" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F35" s="162" t="s">
@@ -16235,31 +16235,31 @@
   <sheetData>
     <row r="2" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B3" s="286"/>
-      <c r="C3" s="287"/>
-      <c r="D3" s="287"/>
-      <c r="E3" s="287"/>
-      <c r="F3" s="287"/>
-      <c r="G3" s="287"/>
-      <c r="H3" s="288"/>
-      <c r="I3" s="292" t="s">
+      <c r="B3" s="288"/>
+      <c r="C3" s="289"/>
+      <c r="D3" s="289"/>
+      <c r="E3" s="289"/>
+      <c r="F3" s="289"/>
+      <c r="G3" s="289"/>
+      <c r="H3" s="290"/>
+      <c r="I3" s="294" t="s">
         <v>74</v>
       </c>
-      <c r="J3" s="293"/>
-      <c r="K3" s="293"/>
-      <c r="L3" s="293"/>
-      <c r="M3" s="293"/>
-      <c r="N3" s="293"/>
-      <c r="O3" s="293"/>
-      <c r="P3" s="293"/>
-      <c r="Q3" s="293"/>
-      <c r="R3" s="293"/>
-      <c r="S3" s="293"/>
-      <c r="T3" s="293"/>
-      <c r="U3" s="293"/>
-      <c r="V3" s="293"/>
-      <c r="W3" s="293"/>
-      <c r="X3" s="294"/>
+      <c r="J3" s="295"/>
+      <c r="K3" s="295"/>
+      <c r="L3" s="295"/>
+      <c r="M3" s="295"/>
+      <c r="N3" s="295"/>
+      <c r="O3" s="295"/>
+      <c r="P3" s="295"/>
+      <c r="Q3" s="295"/>
+      <c r="R3" s="295"/>
+      <c r="S3" s="295"/>
+      <c r="T3" s="295"/>
+      <c r="U3" s="295"/>
+      <c r="V3" s="295"/>
+      <c r="W3" s="295"/>
+      <c r="X3" s="296"/>
       <c r="Y3" s="76"/>
       <c r="Z3" s="51"/>
       <c r="AA3" s="51"/>
@@ -16267,20 +16267,20 @@
       <c r="AC3" s="3"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="1"/>
-      <c r="AF3" s="282"/>
-      <c r="AG3" s="282"/>
-      <c r="AH3" s="282"/>
-      <c r="AI3" s="282"/>
+      <c r="AF3" s="284"/>
+      <c r="AG3" s="284"/>
+      <c r="AH3" s="284"/>
+      <c r="AI3" s="284"/>
       <c r="AJ3" s="1"/>
     </row>
     <row r="4" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B4" s="289"/>
-      <c r="C4" s="290"/>
-      <c r="D4" s="290"/>
-      <c r="E4" s="290"/>
-      <c r="F4" s="290"/>
-      <c r="G4" s="290"/>
-      <c r="H4" s="291"/>
+      <c r="B4" s="291"/>
+      <c r="C4" s="292"/>
+      <c r="D4" s="292"/>
+      <c r="E4" s="292"/>
+      <c r="F4" s="292"/>
+      <c r="G4" s="292"/>
+      <c r="H4" s="293"/>
       <c r="I4" s="52">
         <v>0</v>
       </c>
@@ -16329,7 +16329,7 @@
       <c r="X4" s="53">
         <v>15</v>
       </c>
-      <c r="Y4" s="298" t="s">
+      <c r="Y4" s="300" t="s">
         <v>93</v>
       </c>
       <c r="Z4" s="45"/>
@@ -16348,28 +16348,28 @@
       <c r="B5" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="295" t="s">
+      <c r="C5" s="297" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="296"/>
-      <c r="E5" s="296"/>
-      <c r="F5" s="296"/>
-      <c r="G5" s="296"/>
-      <c r="H5" s="297"/>
-      <c r="I5" s="283" t="s">
+      <c r="D5" s="298"/>
+      <c r="E5" s="298"/>
+      <c r="F5" s="298"/>
+      <c r="G5" s="298"/>
+      <c r="H5" s="299"/>
+      <c r="I5" s="285" t="s">
         <v>77</v>
       </c>
-      <c r="J5" s="284"/>
-      <c r="K5" s="284"/>
-      <c r="L5" s="284"/>
-      <c r="M5" s="284"/>
-      <c r="N5" s="285"/>
-      <c r="O5" s="283" t="s">
+      <c r="J5" s="286"/>
+      <c r="K5" s="286"/>
+      <c r="L5" s="286"/>
+      <c r="M5" s="286"/>
+      <c r="N5" s="287"/>
+      <c r="O5" s="285" t="s">
         <v>78</v>
       </c>
-      <c r="P5" s="284"/>
-      <c r="Q5" s="284"/>
-      <c r="R5" s="285"/>
+      <c r="P5" s="286"/>
+      <c r="Q5" s="286"/>
+      <c r="R5" s="287"/>
       <c r="S5" s="20" t="s">
         <v>79</v>
       </c>
@@ -16388,7 +16388,7 @@
       <c r="X5" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="Y5" s="299"/>
+      <c r="Y5" s="301"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
@@ -22108,14 +22108,14 @@
       </c>
     </row>
     <row r="18" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="D18" s="290" t="s">
+      <c r="D18" s="292" t="s">
         <v>142</v>
       </c>
-      <c r="E18" s="290"/>
-      <c r="G18" s="290" t="s">
+      <c r="E18" s="292"/>
+      <c r="G18" s="292" t="s">
         <v>145</v>
       </c>
-      <c r="H18" s="290"/>
+      <c r="H18" s="292"/>
       <c r="Q18">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Implemented Graphics Memory Instructions
</commit_message>
<xml_diff>
--- a/Documentation/Monty08.xlsx
+++ b/Documentation/Monty08.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\CPU_8Bit\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7D57FE8-E9B1-497C-BBA2-D56538434990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2150A1B5-A360-49A7-812C-48D970D06818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="3585" windowWidth="29040" windowHeight="16440" xr2:uid="{5BA4E079-EFAB-4B55-B322-C6522B3056FF}"/>
+    <workbookView xWindow="38280" yWindow="3585" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{5BA4E079-EFAB-4B55-B322-C6522B3056FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Control-Unit" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="369">
   <si>
     <t>1=Read</t>
   </si>
@@ -1112,6 +1112,45 @@
   </si>
   <si>
     <t>ACC &lt;- PORT</t>
+  </si>
+  <si>
+    <t>PTRREG = #data</t>
+  </si>
+  <si>
+    <t>PTRREG_LOW /HIGH = ACC</t>
+  </si>
+  <si>
+    <t>NIB</t>
+  </si>
+  <si>
+    <t>dat0</t>
+  </si>
+  <si>
+    <t>dat1</t>
+  </si>
+  <si>
+    <t>PSHVB</t>
+  </si>
+  <si>
+    <t>LDPTRV</t>
+  </si>
+  <si>
+    <t>MOVPTRAC</t>
+  </si>
+  <si>
+    <t>GMEM[PTRREG++] = ACC</t>
+  </si>
+  <si>
+    <t>ACC = PTR_LOW/HIGH</t>
+  </si>
+  <si>
+    <t>MOVACPTR</t>
+  </si>
+  <si>
+    <t>G23</t>
+  </si>
+  <si>
+    <t>Write data1 to PTRREG</t>
   </si>
 </sst>
 </file>
@@ -2202,7 +2241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="302">
+  <cellXfs count="304">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2906,6 +2945,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3441,8 +3486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0373F33-972A-4E8D-B1CE-9C5EF0708B27}">
   <dimension ref="A2:AI157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3470,50 +3515,50 @@
     </row>
     <row r="4" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="249" t="s">
+      <c r="C5" s="251" t="s">
         <v>86</v>
       </c>
-      <c r="D5" s="250"/>
-      <c r="E5" s="250"/>
-      <c r="F5" s="250"/>
-      <c r="G5" s="250"/>
-      <c r="H5" s="250"/>
-      <c r="I5" s="250"/>
-      <c r="J5" s="250"/>
-      <c r="K5" s="250"/>
-      <c r="L5" s="251"/>
+      <c r="D5" s="252"/>
+      <c r="E5" s="252"/>
+      <c r="F5" s="252"/>
+      <c r="G5" s="252"/>
+      <c r="H5" s="252"/>
+      <c r="I5" s="252"/>
+      <c r="J5" s="252"/>
+      <c r="K5" s="252"/>
+      <c r="L5" s="253"/>
       <c r="M5" s="123"/>
-      <c r="N5" s="263" t="s">
+      <c r="N5" s="265" t="s">
         <v>85</v>
       </c>
-      <c r="O5" s="263"/>
-      <c r="P5" s="263"/>
-      <c r="Q5" s="263"/>
-      <c r="R5" s="263"/>
-      <c r="S5" s="263"/>
-      <c r="T5" s="263"/>
-      <c r="U5" s="263"/>
-      <c r="V5" s="263"/>
-      <c r="W5" s="263"/>
-      <c r="X5" s="263"/>
-      <c r="Y5" s="263"/>
-      <c r="Z5" s="263"/>
-      <c r="AA5" s="263"/>
-      <c r="AB5" s="263"/>
-      <c r="AC5" s="264"/>
-      <c r="AD5" s="247"/>
+      <c r="O5" s="265"/>
+      <c r="P5" s="265"/>
+      <c r="Q5" s="265"/>
+      <c r="R5" s="265"/>
+      <c r="S5" s="265"/>
+      <c r="T5" s="265"/>
+      <c r="U5" s="265"/>
+      <c r="V5" s="265"/>
+      <c r="W5" s="265"/>
+      <c r="X5" s="265"/>
+      <c r="Y5" s="265"/>
+      <c r="Z5" s="265"/>
+      <c r="AA5" s="265"/>
+      <c r="AB5" s="265"/>
+      <c r="AC5" s="266"/>
+      <c r="AD5" s="249"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="C6" s="252"/>
-      <c r="D6" s="253"/>
-      <c r="E6" s="253"/>
-      <c r="F6" s="253"/>
-      <c r="G6" s="253"/>
-      <c r="H6" s="253"/>
-      <c r="I6" s="253"/>
-      <c r="J6" s="253"/>
-      <c r="K6" s="253"/>
-      <c r="L6" s="254"/>
+      <c r="C6" s="254"/>
+      <c r="D6" s="255"/>
+      <c r="E6" s="255"/>
+      <c r="F6" s="255"/>
+      <c r="G6" s="255"/>
+      <c r="H6" s="255"/>
+      <c r="I6" s="255"/>
+      <c r="J6" s="255"/>
+      <c r="K6" s="255"/>
+      <c r="L6" s="256"/>
       <c r="M6" s="13"/>
       <c r="N6" s="4">
         <v>0</v>
@@ -3563,7 +3608,7 @@
       <c r="AC6" s="124">
         <v>15</v>
       </c>
-      <c r="AD6" s="248"/>
+      <c r="AD6" s="250"/>
       <c r="AE6" s="4"/>
       <c r="AF6" s="4"/>
       <c r="AG6" s="4"/>
@@ -3571,11 +3616,11 @@
       <c r="AI6" s="2"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="C7" s="255"/>
-      <c r="D7" s="256"/>
-      <c r="E7" s="256"/>
-      <c r="F7" s="256"/>
-      <c r="G7" s="256"/>
+      <c r="C7" s="257"/>
+      <c r="D7" s="258"/>
+      <c r="E7" s="258"/>
+      <c r="F7" s="258"/>
+      <c r="G7" s="258"/>
       <c r="H7" s="240"/>
       <c r="I7" s="24" t="s">
         <v>70</v>
@@ -3586,12 +3631,12 @@
       <c r="K7" s="18"/>
       <c r="L7" s="25"/>
       <c r="M7" s="121"/>
-      <c r="N7" s="265"/>
-      <c r="O7" s="265"/>
-      <c r="P7" s="265"/>
-      <c r="Q7" s="265"/>
-      <c r="R7" s="265"/>
-      <c r="S7" s="265"/>
+      <c r="N7" s="267"/>
+      <c r="O7" s="267"/>
+      <c r="P7" s="267"/>
+      <c r="Q7" s="267"/>
+      <c r="R7" s="267"/>
+      <c r="S7" s="267"/>
       <c r="T7" s="5" t="s">
         <v>113</v>
       </c>
@@ -3614,61 +3659,61 @@
       <c r="AA7" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="AB7" s="266" t="s">
+      <c r="AB7" s="268" t="s">
         <v>119</v>
       </c>
-      <c r="AC7" s="267"/>
-      <c r="AD7" s="248"/>
+      <c r="AC7" s="269"/>
+      <c r="AD7" s="250"/>
       <c r="AE7" s="2"/>
       <c r="AF7" s="3"/>
       <c r="AG7" s="3"/>
       <c r="AH7" s="2"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="C8" s="257" t="s">
+      <c r="C8" s="259" t="s">
         <v>329</v>
       </c>
-      <c r="D8" s="258"/>
-      <c r="E8" s="258"/>
-      <c r="F8" s="258"/>
-      <c r="G8" s="258"/>
+      <c r="D8" s="260"/>
+      <c r="E8" s="260"/>
+      <c r="F8" s="260"/>
+      <c r="G8" s="260"/>
       <c r="H8" s="40" t="s">
         <v>348</v>
       </c>
-      <c r="I8" s="259" t="s">
+      <c r="I8" s="261" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="260"/>
-      <c r="K8" s="260"/>
-      <c r="L8" s="261"/>
-      <c r="M8" s="262" t="s">
-        <v>1</v>
-      </c>
-      <c r="N8" s="262"/>
-      <c r="O8" s="262"/>
-      <c r="P8" s="262"/>
-      <c r="Q8" s="262"/>
-      <c r="R8" s="262"/>
-      <c r="S8" s="262"/>
-      <c r="T8" s="271" t="s">
+      <c r="J8" s="262"/>
+      <c r="K8" s="262"/>
+      <c r="L8" s="263"/>
+      <c r="M8" s="264" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="264"/>
+      <c r="O8" s="264"/>
+      <c r="P8" s="264"/>
+      <c r="Q8" s="264"/>
+      <c r="R8" s="264"/>
+      <c r="S8" s="264"/>
+      <c r="T8" s="273" t="s">
         <v>122</v>
       </c>
-      <c r="U8" s="271"/>
-      <c r="V8" s="272" t="s">
+      <c r="U8" s="273"/>
+      <c r="V8" s="274" t="s">
         <v>123</v>
       </c>
-      <c r="W8" s="272"/>
-      <c r="X8" s="272"/>
-      <c r="Y8" s="272"/>
-      <c r="Z8" s="270" t="s">
+      <c r="W8" s="274"/>
+      <c r="X8" s="274"/>
+      <c r="Y8" s="274"/>
+      <c r="Z8" s="272" t="s">
         <v>120</v>
       </c>
-      <c r="AA8" s="270"/>
-      <c r="AB8" s="268" t="s">
+      <c r="AA8" s="272"/>
+      <c r="AB8" s="270" t="s">
         <v>121</v>
       </c>
-      <c r="AC8" s="269"/>
-      <c r="AD8" s="248"/>
+      <c r="AC8" s="271"/>
+      <c r="AD8" s="250"/>
       <c r="AE8" s="118"/>
       <c r="AF8" s="118"/>
       <c r="AG8" s="118"/>
@@ -8358,6 +8403,7 @@
       <c r="F56" s="41"/>
       <c r="G56" s="10"/>
       <c r="H56" s="37"/>
+      <c r="L56" s="17"/>
       <c r="M56" s="13">
         <v>1</v>
       </c>
@@ -8438,6 +8484,7 @@
       <c r="F57" s="41"/>
       <c r="G57" s="10"/>
       <c r="H57" s="37"/>
+      <c r="L57" s="17"/>
       <c r="M57" s="13">
         <v>1</v>
       </c>
@@ -8515,9 +8562,25 @@
       <c r="D58" s="130">
         <v>48</v>
       </c>
-      <c r="F58" s="41"/>
-      <c r="G58" s="10"/>
+      <c r="F58" s="248" t="s">
+        <v>361</v>
+      </c>
+      <c r="G58" s="10" t="s">
+        <v>364</v>
+      </c>
       <c r="H58" s="37"/>
+      <c r="I58" s="17">
+        <v>0</v>
+      </c>
+      <c r="J58" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="K58" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="L58" s="17" t="s">
+        <v>67</v>
+      </c>
       <c r="M58" s="13">
         <v>1</v>
       </c>
@@ -8543,7 +8606,7 @@
         <v>1</v>
       </c>
       <c r="U58" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V58" s="40">
         <v>1</v>
@@ -8571,7 +8634,7 @@
       </c>
       <c r="AD58" s="173" t="str">
         <f t="shared" si="21"/>
-        <v>CBC0</v>
+        <v>CB40</v>
       </c>
       <c r="AE58" s="3" t="str">
         <f t="shared" si="22"/>
@@ -8579,7 +8642,7 @@
       </c>
       <c r="AF58" s="2" t="str">
         <f t="shared" si="23"/>
-        <v>C0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="59" spans="1:32" x14ac:dyDescent="0.25">
@@ -8595,33 +8658,51 @@
       <c r="D59" s="130">
         <v>49</v>
       </c>
-      <c r="F59" s="41"/>
-      <c r="G59" s="10"/>
+      <c r="E59" s="40" t="s">
+        <v>367</v>
+      </c>
+      <c r="F59" s="248" t="s">
+        <v>362</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>356</v>
+      </c>
       <c r="H59" s="37"/>
-      <c r="L59" s="11"/>
+      <c r="I59" s="17">
+        <v>0</v>
+      </c>
+      <c r="J59" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="K59" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="L59" s="17" t="s">
+        <v>360</v>
+      </c>
       <c r="M59" s="13">
         <v>1</v>
       </c>
       <c r="N59" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O59" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P59" s="40">
         <v>0</v>
       </c>
       <c r="Q59" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R59" s="40">
         <v>0</v>
       </c>
       <c r="S59" s="41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T59" s="40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U59" s="41">
         <v>1</v>
@@ -8639,7 +8720,7 @@
         <v>1</v>
       </c>
       <c r="Z59" s="40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA59" s="41">
         <v>0</v>
@@ -8652,15 +8733,15 @@
       </c>
       <c r="AD59" s="173" t="str">
         <f t="shared" ref="AD59" si="27">_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(AC59,AB59,AA59,Z59)), BIN2HEX(_xlfn.CONCAT(Y59,X59,W59,V59)), BIN2HEX(_xlfn.CONCAT(U59,T59,S59,R59)), BIN2HEX(_xlfn.CONCAT(Q59,P59,O59,N59)))</f>
-        <v>CBC0</v>
+        <v>DBAB</v>
       </c>
       <c r="AE59" s="3" t="str">
         <f t="shared" ref="AE59" si="28">_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(AC59,AB59,AA59,Z59)), BIN2HEX(_xlfn.CONCAT(Y59,X59,W59,V59)))</f>
-        <v>CB</v>
+        <v>DB</v>
       </c>
       <c r="AF59" s="2" t="str">
         <f t="shared" ref="AF59" si="29">_xlfn.CONCAT(BIN2HEX(_xlfn.CONCAT(U59,T59,S59,R59)),BIN2HEX(_xlfn.CONCAT(Q59,P59,O59,N59)))</f>
-        <v>C0</v>
+        <v>AB</v>
       </c>
     </row>
     <row r="60" spans="1:32" x14ac:dyDescent="0.25">
@@ -8676,10 +8757,25 @@
       <c r="D60" s="130">
         <v>50</v>
       </c>
-      <c r="F60" s="41"/>
-      <c r="G60" s="10"/>
+      <c r="F60" s="247" t="s">
+        <v>363</v>
+      </c>
+      <c r="G60" s="10" t="s">
+        <v>357</v>
+      </c>
       <c r="H60" s="37"/>
-      <c r="L60" s="11"/>
+      <c r="I60" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="J60" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="K60" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="L60" s="17" t="s">
+        <v>67</v>
+      </c>
       <c r="M60" s="13">
         <v>1</v>
       </c>
@@ -8705,7 +8801,7 @@
         <v>1</v>
       </c>
       <c r="U60" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V60" s="40">
         <v>1</v>
@@ -8733,7 +8829,7 @@
       </c>
       <c r="AD60" s="173" t="str">
         <f t="shared" si="1"/>
-        <v>CBC0</v>
+        <v>CB40</v>
       </c>
       <c r="AE60" s="3" t="str">
         <f t="shared" si="2"/>
@@ -8741,7 +8837,7 @@
       </c>
       <c r="AF60" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>C0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="61" spans="1:32" x14ac:dyDescent="0.25">
@@ -8757,10 +8853,25 @@
       <c r="D61" s="130">
         <v>51</v>
       </c>
-      <c r="F61" s="41"/>
-      <c r="G61" s="10"/>
+      <c r="F61" s="247" t="s">
+        <v>366</v>
+      </c>
+      <c r="G61" s="10" t="s">
+        <v>365</v>
+      </c>
       <c r="H61" s="37"/>
-      <c r="L61" s="11"/>
+      <c r="I61" s="17" t="s">
+        <v>358</v>
+      </c>
+      <c r="J61" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="K61" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="L61" s="17" t="s">
+        <v>67</v>
+      </c>
       <c r="M61" s="13">
         <v>1</v>
       </c>
@@ -8786,13 +8897,13 @@
         <v>1</v>
       </c>
       <c r="U61" s="41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V61" s="40">
         <v>1</v>
       </c>
       <c r="W61" s="40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X61" s="40">
         <v>0</v>
@@ -8814,15 +8925,15 @@
       </c>
       <c r="AD61" s="173" t="str">
         <f t="shared" si="1"/>
-        <v>CBC0</v>
+        <v>C940</v>
       </c>
       <c r="AE61" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>CB</v>
+        <v>C9</v>
       </c>
       <c r="AF61" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>C0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="62" spans="1:32" x14ac:dyDescent="0.25">
@@ -14274,8 +14385,12 @@
       <c r="D127" s="130">
         <v>117</v>
       </c>
-      <c r="F127" s="41"/>
-      <c r="G127" s="10"/>
+      <c r="F127" s="41" t="s">
+        <v>367</v>
+      </c>
+      <c r="G127" s="10" t="s">
+        <v>368</v>
+      </c>
       <c r="H127" s="10"/>
       <c r="L127" s="9"/>
       <c r="M127" s="41">
@@ -14299,27 +14414,47 @@
       <c r="S127" s="40">
         <v>0</v>
       </c>
-      <c r="T127" s="40"/>
-      <c r="U127" s="41"/>
-      <c r="V127" s="40"/>
-      <c r="W127" s="40"/>
-      <c r="X127" s="40"/>
-      <c r="Y127" s="41"/>
-      <c r="Z127" s="40"/>
-      <c r="AA127" s="41"/>
-      <c r="AB127" s="40"/>
-      <c r="AC127" s="134"/>
+      <c r="T127" s="40">
+        <v>0</v>
+      </c>
+      <c r="U127" s="41">
+        <v>1</v>
+      </c>
+      <c r="V127" s="40">
+        <v>1</v>
+      </c>
+      <c r="W127" s="40">
+        <v>1</v>
+      </c>
+      <c r="X127" s="40">
+        <v>0</v>
+      </c>
+      <c r="Y127" s="41">
+        <v>1</v>
+      </c>
+      <c r="Z127" s="40">
+        <v>1</v>
+      </c>
+      <c r="AA127" s="41">
+        <v>0</v>
+      </c>
+      <c r="AB127" s="40">
+        <v>1</v>
+      </c>
+      <c r="AC127" s="134">
+        <v>1</v>
+      </c>
       <c r="AD127" s="173" t="str">
         <f t="shared" si="41"/>
-        <v>0000</v>
+        <v>DB80</v>
       </c>
       <c r="AE127" s="3" t="str">
         <f t="shared" si="42"/>
-        <v>00</v>
+        <v>DB</v>
       </c>
       <c r="AF127" s="2" t="str">
         <f t="shared" si="43"/>
-        <v>00</v>
+        <v>80</v>
       </c>
     </row>
     <row r="128" spans="2:32" x14ac:dyDescent="0.25">
@@ -15122,61 +15257,61 @@
       <c r="F5" s="163" t="s">
         <v>209</v>
       </c>
-      <c r="G5" s="273" t="s">
+      <c r="G5" s="275" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="6" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F6" s="162"/>
-      <c r="G6" s="274"/>
+      <c r="G6" s="276"/>
     </row>
     <row r="7" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F7" s="162"/>
-      <c r="G7" s="274"/>
+      <c r="G7" s="276"/>
     </row>
     <row r="8" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F8" s="162"/>
-      <c r="G8" s="274"/>
+      <c r="G8" s="276"/>
     </row>
     <row r="9" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F9" s="162"/>
-      <c r="G9" s="274"/>
+      <c r="G9" s="276"/>
     </row>
     <row r="10" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F10" s="162"/>
-      <c r="G10" s="274"/>
+      <c r="G10" s="276"/>
     </row>
     <row r="11" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F11" s="162"/>
-      <c r="G11" s="274"/>
+      <c r="G11" s="276"/>
     </row>
     <row r="12" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F12" s="162"/>
-      <c r="G12" s="274"/>
+      <c r="G12" s="276"/>
     </row>
     <row r="13" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F13" s="162"/>
-      <c r="G13" s="274"/>
+      <c r="G13" s="276"/>
     </row>
     <row r="14" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F14" s="162"/>
-      <c r="G14" s="274"/>
+      <c r="G14" s="276"/>
     </row>
     <row r="15" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F15" s="162"/>
-      <c r="G15" s="274"/>
+      <c r="G15" s="276"/>
     </row>
     <row r="16" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F16" s="164" t="s">
         <v>213</v>
       </c>
-      <c r="G16" s="275"/>
+      <c r="G16" s="277"/>
     </row>
     <row r="17" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F17" s="162" t="s">
         <v>210</v>
       </c>
-      <c r="G17" s="276" t="s">
+      <c r="G17" s="278" t="s">
         <v>212</v>
       </c>
     </row>
@@ -15184,83 +15319,83 @@
       <c r="F18" s="164" t="s">
         <v>214</v>
       </c>
-      <c r="G18" s="277"/>
+      <c r="G18" s="279"/>
     </row>
     <row r="19" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F19" s="162" t="s">
         <v>215</v>
       </c>
-      <c r="G19" s="278" t="s">
+      <c r="G19" s="280" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="20" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F20" s="162"/>
-      <c r="G20" s="279"/>
+      <c r="G20" s="281"/>
     </row>
     <row r="21" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F21" s="162"/>
-      <c r="G21" s="279"/>
+      <c r="G21" s="281"/>
     </row>
     <row r="22" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F22" s="164" t="s">
         <v>216</v>
       </c>
-      <c r="G22" s="280"/>
+      <c r="G22" s="282"/>
     </row>
     <row r="23" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F23" s="162" t="s">
         <v>218</v>
       </c>
-      <c r="G23" s="281" t="s">
+      <c r="G23" s="283" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="24" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F24" s="162"/>
-      <c r="G24" s="282"/>
+      <c r="G24" s="284"/>
     </row>
     <row r="25" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F25" s="162"/>
-      <c r="G25" s="282"/>
+      <c r="G25" s="284"/>
     </row>
     <row r="26" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F26" s="162"/>
-      <c r="G26" s="282"/>
+      <c r="G26" s="284"/>
     </row>
     <row r="27" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F27" s="162"/>
-      <c r="G27" s="282"/>
+      <c r="G27" s="284"/>
     </row>
     <row r="28" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F28" s="162"/>
-      <c r="G28" s="282"/>
+      <c r="G28" s="284"/>
     </row>
     <row r="29" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F29" s="162"/>
-      <c r="G29" s="282"/>
+      <c r="G29" s="284"/>
     </row>
     <row r="30" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F30" s="162"/>
-      <c r="G30" s="282"/>
+      <c r="G30" s="284"/>
     </row>
     <row r="31" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F31" s="162"/>
-      <c r="G31" s="282"/>
+      <c r="G31" s="284"/>
     </row>
     <row r="32" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F32" s="162"/>
-      <c r="G32" s="282"/>
+      <c r="G32" s="284"/>
     </row>
     <row r="33" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F33" s="162"/>
-      <c r="G33" s="282"/>
+      <c r="G33" s="284"/>
     </row>
     <row r="34" spans="6:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F34" s="164" t="s">
         <v>219</v>
       </c>
-      <c r="G34" s="283"/>
+      <c r="G34" s="285"/>
     </row>
     <row r="35" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F35" s="162" t="s">
@@ -16235,31 +16370,31 @@
   <sheetData>
     <row r="2" spans="2:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B3" s="288"/>
-      <c r="C3" s="289"/>
-      <c r="D3" s="289"/>
-      <c r="E3" s="289"/>
-      <c r="F3" s="289"/>
-      <c r="G3" s="289"/>
-      <c r="H3" s="290"/>
-      <c r="I3" s="294" t="s">
+      <c r="B3" s="290"/>
+      <c r="C3" s="291"/>
+      <c r="D3" s="291"/>
+      <c r="E3" s="291"/>
+      <c r="F3" s="291"/>
+      <c r="G3" s="291"/>
+      <c r="H3" s="292"/>
+      <c r="I3" s="296" t="s">
         <v>74</v>
       </c>
-      <c r="J3" s="295"/>
-      <c r="K3" s="295"/>
-      <c r="L3" s="295"/>
-      <c r="M3" s="295"/>
-      <c r="N3" s="295"/>
-      <c r="O3" s="295"/>
-      <c r="P3" s="295"/>
-      <c r="Q3" s="295"/>
-      <c r="R3" s="295"/>
-      <c r="S3" s="295"/>
-      <c r="T3" s="295"/>
-      <c r="U3" s="295"/>
-      <c r="V3" s="295"/>
-      <c r="W3" s="295"/>
-      <c r="X3" s="296"/>
+      <c r="J3" s="297"/>
+      <c r="K3" s="297"/>
+      <c r="L3" s="297"/>
+      <c r="M3" s="297"/>
+      <c r="N3" s="297"/>
+      <c r="O3" s="297"/>
+      <c r="P3" s="297"/>
+      <c r="Q3" s="297"/>
+      <c r="R3" s="297"/>
+      <c r="S3" s="297"/>
+      <c r="T3" s="297"/>
+      <c r="U3" s="297"/>
+      <c r="V3" s="297"/>
+      <c r="W3" s="297"/>
+      <c r="X3" s="298"/>
       <c r="Y3" s="76"/>
       <c r="Z3" s="51"/>
       <c r="AA3" s="51"/>
@@ -16267,20 +16402,20 @@
       <c r="AC3" s="3"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="1"/>
-      <c r="AF3" s="284"/>
-      <c r="AG3" s="284"/>
-      <c r="AH3" s="284"/>
-      <c r="AI3" s="284"/>
+      <c r="AF3" s="286"/>
+      <c r="AG3" s="286"/>
+      <c r="AH3" s="286"/>
+      <c r="AI3" s="286"/>
       <c r="AJ3" s="1"/>
     </row>
     <row r="4" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B4" s="291"/>
-      <c r="C4" s="292"/>
-      <c r="D4" s="292"/>
-      <c r="E4" s="292"/>
-      <c r="F4" s="292"/>
-      <c r="G4" s="292"/>
-      <c r="H4" s="293"/>
+      <c r="B4" s="293"/>
+      <c r="C4" s="294"/>
+      <c r="D4" s="294"/>
+      <c r="E4" s="294"/>
+      <c r="F4" s="294"/>
+      <c r="G4" s="294"/>
+      <c r="H4" s="295"/>
       <c r="I4" s="52">
         <v>0</v>
       </c>
@@ -16329,7 +16464,7 @@
       <c r="X4" s="53">
         <v>15</v>
       </c>
-      <c r="Y4" s="300" t="s">
+      <c r="Y4" s="302" t="s">
         <v>93</v>
       </c>
       <c r="Z4" s="45"/>
@@ -16348,28 +16483,28 @@
       <c r="B5" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="297" t="s">
+      <c r="C5" s="299" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="298"/>
-      <c r="E5" s="298"/>
-      <c r="F5" s="298"/>
-      <c r="G5" s="298"/>
-      <c r="H5" s="299"/>
-      <c r="I5" s="285" t="s">
+      <c r="D5" s="300"/>
+      <c r="E5" s="300"/>
+      <c r="F5" s="300"/>
+      <c r="G5" s="300"/>
+      <c r="H5" s="301"/>
+      <c r="I5" s="287" t="s">
         <v>77</v>
       </c>
-      <c r="J5" s="286"/>
-      <c r="K5" s="286"/>
-      <c r="L5" s="286"/>
-      <c r="M5" s="286"/>
-      <c r="N5" s="287"/>
-      <c r="O5" s="285" t="s">
+      <c r="J5" s="288"/>
+      <c r="K5" s="288"/>
+      <c r="L5" s="288"/>
+      <c r="M5" s="288"/>
+      <c r="N5" s="289"/>
+      <c r="O5" s="287" t="s">
         <v>78</v>
       </c>
-      <c r="P5" s="286"/>
-      <c r="Q5" s="286"/>
-      <c r="R5" s="287"/>
+      <c r="P5" s="288"/>
+      <c r="Q5" s="288"/>
+      <c r="R5" s="289"/>
       <c r="S5" s="20" t="s">
         <v>79</v>
       </c>
@@ -16388,7 +16523,7 @@
       <c r="X5" s="55" t="s">
         <v>88</v>
       </c>
-      <c r="Y5" s="301"/>
+      <c r="Y5" s="303"/>
       <c r="Z5" s="3"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
@@ -21597,8 +21732,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F461F9F-87D6-4C96-820F-6111A3E2F850}">
   <dimension ref="C4:AA37"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22108,14 +22243,14 @@
       </c>
     </row>
     <row r="18" spans="3:27" x14ac:dyDescent="0.25">
-      <c r="D18" s="292" t="s">
+      <c r="D18" s="294" t="s">
         <v>142</v>
       </c>
-      <c r="E18" s="292"/>
-      <c r="G18" s="292" t="s">
+      <c r="E18" s="294"/>
+      <c r="G18" s="294" t="s">
         <v>145</v>
       </c>
-      <c r="H18" s="292"/>
+      <c r="H18" s="294"/>
       <c r="Q18">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
Tested Video Memory Instructions
</commit_message>
<xml_diff>
--- a/Documentation/Monty08.xlsx
+++ b/Documentation/Monty08.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\CPU_8Bit\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2150A1B5-A360-49A7-812C-48D970D06818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA3E176-2C40-400A-9CAE-2917DA7F748F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="3585" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{5BA4E079-EFAB-4B55-B322-C6522B3056FF}"/>
+    <workbookView xWindow="38280" yWindow="3585" windowWidth="29040" windowHeight="16440" xr2:uid="{5BA4E079-EFAB-4B55-B322-C6522B3056FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Control-Unit" sheetId="1" r:id="rId1"/>
@@ -3486,8 +3486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0373F33-972A-4E8D-B1CE-9C5EF0708B27}">
   <dimension ref="A2:AI157"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K59" sqref="K59"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M50" sqref="M50:N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8550,7 +8550,7 @@
       </c>
     </row>
     <row r="58" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A58" s="178"/>
+      <c r="A58" s="160"/>
       <c r="B58" s="40" t="str">
         <f t="shared" si="24"/>
         <v>30</v>
@@ -8646,7 +8646,7 @@
       </c>
     </row>
     <row r="59" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A59" s="178"/>
+      <c r="A59" s="160"/>
       <c r="B59" s="40" t="str">
         <f t="shared" ref="B59:B67" si="25">DEC2HEX(D59)</f>
         <v>31</v>
@@ -8745,7 +8745,7 @@
       </c>
     </row>
     <row r="60" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A60" s="178"/>
+      <c r="A60" s="160"/>
       <c r="B60" s="40" t="str">
         <f t="shared" si="25"/>
         <v>32</v>
@@ -8841,7 +8841,7 @@
       </c>
     </row>
     <row r="61" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A61" s="178"/>
+      <c r="A61" s="160"/>
       <c r="B61" s="40" t="str">
         <f t="shared" si="25"/>
         <v>33</v>
@@ -21732,7 +21732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F461F9F-87D6-4C96-820F-6111A3E2F850}">
   <dimension ref="C4:AA37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>

</xml_diff>